<commit_message>
added timemismatch and removed debug prints
</commit_message>
<xml_diff>
--- a/output/children_surveys.xlsx
+++ b/output/children_surveys.xlsx
@@ -32,7 +32,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -75,6 +75,12 @@
         <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCFF"/>
+        <bgColor rgb="00CCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -94,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -113,6 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -2628,7 +2635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ668"/>
+  <dimension ref="A1:AJ669"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -75002,6 +75009,13 @@
         </is>
       </c>
     </row>
+    <row r="669">
+      <c r="A669" s="16" t="inlineStr">
+        <is>
+          <t>time_mismatch</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>

</xml_diff>